<commit_message>
rewrote backend logic for cohort and rewort cohort test for both rasa and python unit
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2014_2015.xlsx
+++ b/CDSData/CDS_SPARSE_2014_2015.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87428751-7E29-400D-9F9A-B5622D6F42CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85F6B5A-AA94-4BD9-A202-6233CCA041B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,22 +42,7 @@
     <t>any-aid</t>
   </si>
   <si>
-    <t>within-4-years</t>
-  </si>
-  <si>
-    <t>4-5-years</t>
-  </si>
-  <si>
-    <t>5-6-years</t>
-  </si>
-  <si>
-    <t>total-graduated</t>
-  </si>
-  <si>
     <t>exemptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6-year graduation-rate</t>
   </si>
   <si>
     <t>initial</t>
@@ -67,6 +52,21 @@
   </si>
   <si>
     <t>stafford-loan</t>
+  </si>
+  <si>
+    <t>within</t>
+  </si>
+  <si>
+    <t>between</t>
+  </si>
+  <si>
+    <t>5 year</t>
+  </si>
+  <si>
+    <t>4 year</t>
+  </si>
+  <si>
+    <t>6 year</t>
   </si>
 </sst>
 </file>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -413,12 +413,10 @@
     <col min="5" max="5" width="15.109375" customWidth="1"/>
     <col min="6" max="6" width="11.88671875" customWidth="1"/>
     <col min="7" max="7" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" customWidth="1"/>
-    <col min="11" max="11" width="14.21875" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" customWidth="1"/>
-    <col min="13" max="13" width="19.88671875" customWidth="1"/>
+    <col min="8" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+    <col min="13" max="13" width="14.21875" customWidth="1"/>
     <col min="14" max="14" width="10.88671875" customWidth="1"/>
     <col min="15" max="15" width="11.109375" customWidth="1"/>
   </cols>
@@ -431,7 +429,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -443,28 +441,28 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
         <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -1020,14 +1018,14 @@
       <c r="H14" s="2">
         <v>0</v>
       </c>
-      <c r="I14">
-        <v>1</v>
+      <c r="I14" s="2">
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -1065,13 +1063,13 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1108,14 +1106,14 @@
       <c r="H16" s="2">
         <v>0</v>
       </c>
-      <c r="I16">
-        <v>1</v>
+      <c r="I16" s="2">
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -1152,14 +1150,14 @@
       <c r="H17" s="2">
         <v>0</v>
       </c>
-      <c r="I17">
-        <v>1</v>
+      <c r="I17" s="2">
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -1196,17 +1194,17 @@
       <c r="H18" s="2">
         <v>0</v>
       </c>
-      <c r="I18">
-        <v>0</v>
+      <c r="I18" s="2">
+        <v>1</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -1240,17 +1238,17 @@
       <c r="H19" s="2">
         <v>0</v>
       </c>
-      <c r="I19">
-        <v>0</v>
+      <c r="I19" s="2">
+        <v>1</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -1284,17 +1282,17 @@
       <c r="H20" s="2">
         <v>0</v>
       </c>
-      <c r="I20">
-        <v>0</v>
+      <c r="I20" s="2">
+        <v>1</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -1328,17 +1326,17 @@
       <c r="H21" s="2">
         <v>0</v>
       </c>
-      <c r="I21">
-        <v>0</v>
+      <c r="I21" s="2">
+        <v>1</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21">
         <v>0</v>
@@ -1372,20 +1370,20 @@
       <c r="H22" s="2">
         <v>0</v>
       </c>
-      <c r="I22">
-        <v>0</v>
+      <c r="I22" s="2">
+        <v>1</v>
       </c>
       <c r="J22">
         <v>0</v>
       </c>
       <c r="K22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -1416,20 +1414,20 @@
       <c r="H23" s="2">
         <v>0</v>
       </c>
-      <c r="I23">
-        <v>0</v>
+      <c r="I23" s="2">
+        <v>1</v>
       </c>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -1460,20 +1458,20 @@
       <c r="H24" s="2">
         <v>0</v>
       </c>
-      <c r="I24">
-        <v>0</v>
+      <c r="I24" s="2">
+        <v>1</v>
       </c>
       <c r="J24">
         <v>0</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -1504,379 +1502,29 @@
       <c r="H25" s="2">
         <v>0</v>
       </c>
-      <c r="I25">
-        <v>0</v>
+      <c r="I25" s="2">
+        <v>1</v>
       </c>
       <c r="J25">
         <v>0</v>
       </c>
       <c r="K25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>69</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>1</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>158</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27" s="2">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>1</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>256</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" s="2">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28" s="2">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>1</v>
-      </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>483</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29" s="2">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29" s="2">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>1</v>
-      </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>83</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2">
-        <v>0</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <v>1</v>
-      </c>
-      <c r="N30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>79</v>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31">
-        <v>1</v>
-      </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>85.6</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-      <c r="M32">
-        <v>1</v>
-      </c>
-      <c r="N32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>83</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33" s="2">
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33" s="2">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="M33">
-        <v>1</v>
-      </c>
-      <c r="N33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="H34" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>